<commit_message>
Second commit, working code.
</commit_message>
<xml_diff>
--- a/EmployeeSQL/table_layout.xlsx
+++ b/EmployeeSQL/table_layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Homework9\sql-challenge\EmployeeSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3F13EE3-1161-4E3F-87C5-0C2FAECAC1C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCF21F0-B590-44FE-9329-87B32DD85FC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="876" windowWidth="18048" windowHeight="9816" xr2:uid="{BFBDEF07-34ED-4C3E-9F0A-25920B872F59}"/>
+    <workbookView xWindow="1752" yWindow="876" windowWidth="12792" windowHeight="10944" xr2:uid="{BFBDEF07-34ED-4C3E-9F0A-25920B872F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>dept_no</t>
   </si>
@@ -47,9 +47,6 @@
     <t>departments</t>
   </si>
   <si>
-    <t>dept employee</t>
-  </si>
-  <si>
     <t>emp_no</t>
   </si>
   <si>
@@ -105,6 +102,54 @@
   </si>
   <si>
     <t>titles</t>
+  </si>
+  <si>
+    <t>dept_name VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>dept_employee</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>emp_no INT Not NULL PK</t>
+  </si>
+  <si>
+    <t>dept_no VARCHAR(20) PK</t>
+  </si>
+  <si>
+    <t>from_date VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>to_date VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>emp_no INT Not NULL FK -dept_employee.emp_no</t>
+  </si>
+  <si>
+    <t>birth_date VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>first_name VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>last_name VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>gender VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>hire_date VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>salary INT</t>
+  </si>
+  <si>
+    <t>title VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>dept_no VARCHAR(20) FK -departments.dept_no</t>
   </si>
 </sst>
 </file>
@@ -457,234 +502,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F23258-7308-435C-BE95-D2F47F49F5CB}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B8">
+        <v>10001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>31589</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2958101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>110022</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1">
+        <v>31048</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>33512</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
         <v>10001</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>19604</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="1">
+        <v>31589</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>10001</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32">
+        <v>60117</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="B33" s="1">
         <v>31589</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2958101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>110022</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1">
-        <v>31048</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1">
-        <v>33512</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>10001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1">
-        <v>19604</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1">
-        <v>31589</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26">
-        <v>10001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27">
-        <v>60117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="1">
-        <v>31589</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="1">
-        <v>31954</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>10001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="1">
+        <v>31954</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>10001</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="1">
         <v>31589</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="1">
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="1">
         <v>2958101</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>